<commit_message>
dodělání experimentu acrobot-v0 + výsledků na analýzu
</commit_message>
<xml_diff>
--- a/Bakalarska_prace/test_001/Tabulky výsledků.xlsx
+++ b/Bakalarska_prace/test_001/Tabulky výsledků.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LachubCz_NTB\Documents\GitHub\VUT-FIT\Bakalarska_prace\ObecnyAlgoritmus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LachubCz_NTB\Documents\GitHub\VUT-FIT\Bakalarska_prace\test_001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CEF8F6-BCE2-423A-9A4E-6B752FAF8EC2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1866DDD5-54A6-437F-BA24-EA70F5D5A89F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3" xr2:uid="{E4439C24-0DB8-410B-B158-614BB7550185}"/>
   </bookViews>
@@ -4253,7 +4253,7 @@
                   <c:v>-210.60600000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-289.86750000000001</c:v>
+                  <c:v>-331.89400000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>-227.506</c:v>
@@ -10645,8 +10645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93D63314-D5A8-44DB-83D9-D4C6CFD9D269}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10738,13 +10738,16 @@
       <c r="D6">
         <v>-475.99</v>
       </c>
+      <c r="E6">
+        <v>-500</v>
+      </c>
       <c r="G6">
         <f t="shared" ref="G6" si="2">AVERAGE(A6:E6)</f>
-        <v>-289.86750000000001</v>
+        <v>-331.89400000000001</v>
       </c>
       <c r="H6">
         <f t="shared" ref="H6" si="3">_xlfn.STDEV.P(A6:E6)</f>
-        <v>196.25453833924453</v>
+        <v>194.62163770763004</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -10934,7 +10937,7 @@
       </c>
       <c r="C18">
         <f>G6</f>
-        <v>-289.86750000000001</v>
+        <v>-331.89400000000001</v>
       </c>
       <c r="D18">
         <f>G8</f>
@@ -10968,7 +10971,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="14"/>
-        <v>41.069626639757828</v>
+        <v>48.531760140285755</v>
       </c>
       <c r="D20">
         <f t="shared" si="14"/>

</xml_diff>